<commit_message>
Inclusão da apresentação sobre conceitos básicos
</commit_message>
<xml_diff>
--- a/dados/SacoGrandeII.xlsx
+++ b/dados/SacoGrandeII.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilberto\OneDrive\Documentos\1sem2015\sociais\ConceitosBasicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilberto\OneDrive\Documentos\pagina\gpsassi.github.io\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="21">
   <si>
     <t>Grau de Instrução do chefe de família</t>
   </si>
@@ -86,6 +86,9 @@
   <si>
     <t>Grau de Instrução</t>
   </si>
+  <si>
+    <t>Família</t>
+  </si>
 </sst>
 </file>
 
@@ -133,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -332,26 +335,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -369,18 +391,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -390,6 +400,30 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -399,11 +433,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,7 +660,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Dados Brutos'!$D$6:$D$8</c:f>
+              <c:f>'Dados Brutos'!$E$6:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -643,7 +677,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Dados Brutos'!$E$6:$E$8</c:f>
+              <c:f>'Dados Brutos'!$F$6:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1112,7 +1146,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1269,9 +1302,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1332,7 +1363,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1439,7 +1469,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1596,9 +1625,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1659,7 +1686,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3958,13 +3984,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
@@ -4347,1221 +4373,1703 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="str">
-        <f>B2</f>
+      <c r="C3" s="2" t="str">
+        <f>C2</f>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="str">
-        <f t="shared" ref="B4:B41" si="0">B3</f>
+      <c r="C4" s="2" t="str">
+        <f t="shared" ref="C4:C41" si="1">C3</f>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="str">
+      <c r="B5" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="27"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="12">
+        <f>COUNTIF(B2:B121,"Nenhum Grau Completo")</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="8">
+        <f>COUNTIF(B2:B121,"Primeiro Grau Completo")</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="8">
+        <f>COUNTIF(B2:B121,"Segundo Grau Completo")</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="str">
+      <c r="B9" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="10">
+        <f xml:space="preserve"> SUM(F6:F8)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D6" s="14" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="15">
-        <f>COUNTIF(A2:A121,"Nenhum Grau Completo")</f>
+      <c r="F20" s="15">
+        <f>COUNTIF(B2:B121,"Nenhum Grau Completo")</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="str">
+      <c r="G20" s="17">
+        <f>F20/F23</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="H20" s="13">
+        <f>G20*100</f>
+        <v>31.666666666666664</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="11">
-        <f>COUNTIF(A2:A121,"Primeiro Grau Completo")</f>
+      <c r="F21" s="15">
+        <f>COUNTIF(B2:B121,"Primeiro Grau Completo")</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="str">
+      <c r="G21" s="17">
+        <f>F21/F23</f>
+        <v>0.30833333333333335</v>
+      </c>
+      <c r="H21" s="13">
+        <f>G21*100</f>
+        <v>30.833333333333336</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="11">
-        <f>COUNTIF(A2:A121,"Segundo Grau Completo")</f>
+      <c r="F22" s="15">
+        <f>COUNTIF(B2:B121,"Segundo Grau Completo")</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="str">
+      <c r="G22" s="17">
+        <f>F22/F23</f>
+        <v>0.375</v>
+      </c>
+      <c r="H22" s="13">
+        <f>G22*100</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
         <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="E23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="13">
-        <f xml:space="preserve"> SUM(E6:E8)</f>
+      <c r="F23" s="16">
+        <f xml:space="preserve"> SUM(F20:F22)</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3" t="str">
+      <c r="G23" s="18">
+        <f>SUM(G20:G22)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="19">
+        <f xml:space="preserve"> SUM(H20:H22)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3" t="str">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3" t="str">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3" t="str">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3" t="str">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="3" t="str">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3" t="str">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="3" t="str">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3" t="str">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D18" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="3" t="str">
+      <c r="C33" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="3" t="str">
+      <c r="C35" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="22">
-        <f>COUNTIF(A2:A121,"Nenhum Grau Completo")</f>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F20" s="24">
-        <f>E20/E23</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="G20" s="20">
-        <f>F20*100</f>
-        <v>31.666666666666664</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B39" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="3" t="str">
+      <c r="C39" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="1"/>
         <v>Conjunto Residencial Monte Verde</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="22">
-        <f>COUNTIF(A2:A121,"Primeiro Grau Completo")</f>
-        <v>37</v>
-      </c>
-      <c r="F21" s="24">
-        <f>E21/E23</f>
-        <v>0.30833333333333335</v>
-      </c>
-      <c r="G21" s="20">
-        <f>F21*100</f>
-        <v>30.833333333333336</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="3" t="str">
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Conjunto Residencial Monte Verde</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="22">
-        <f>COUNTIF(A2:A121,"Segundo Grau Completo")</f>
-        <v>45</v>
-      </c>
-      <c r="F22" s="24">
-        <f>E22/E23</f>
-        <v>0.375</v>
-      </c>
-      <c r="G22" s="20">
-        <f>F22*100</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="3" t="str">
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="23">
-        <f xml:space="preserve"> SUM(E20:E22)</f>
-        <v>120</v>
-      </c>
-      <c r="F23" s="25">
-        <f>SUM(F20:F22)</f>
-        <v>1</v>
-      </c>
-      <c r="G23" s="26">
-        <f xml:space="preserve"> SUM(G20:G22)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="3" t="str">
+      <c r="C43" s="2" t="str">
+        <f>C42</f>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="3" t="str">
+      <c r="C44" s="2" t="str">
+        <f t="shared" ref="C44:C56" si="2">C43</f>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Conjunto Residencial Monte Verde</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="3" t="str">
-        <f>B42</f>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="3" t="str">
-        <f t="shared" ref="B44:B56" si="1">B43</f>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57" s="3" t="str">
-        <f>B56</f>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58" s="3" t="str">
-        <f t="shared" ref="B58:B70" si="2">B57</f>
-        <v>Conjunto Residencial Pq da Figureira</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B59" s="3" t="str">
+      <c r="C45" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="3" t="str">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B61" s="3" t="str">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" s="3" t="str">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B63" s="3" t="str">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="3" t="str">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B65" s="3" t="str">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66" s="3" t="str">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B67" s="3" t="str">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68" s="3" t="str">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B69" s="3" t="str">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="3" t="str">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="3" t="str">
-        <f>B70</f>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="2" t="str">
+        <f>C56</f>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" s="3" t="str">
-        <f t="shared" ref="B72:B84" si="3">B71</f>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="2" t="str">
+        <f t="shared" ref="C58:C70" si="3">C57</f>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="3" t="str">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B74" s="3" t="str">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B75" s="3" t="str">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" s="3" t="str">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="3" t="str">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B78" s="3" t="str">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B79" s="3" t="str">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="3" t="str">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B81" s="3" t="str">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="3" t="str">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
+        <f t="shared" ref="A68:A121" si="4">A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B83" s="3" t="str">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B84" s="3" t="str">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <f t="shared" si="4"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="2" t="str">
         <f t="shared" si="3"/>
         <v>Conjunto Residencial Pq da Figureira</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="2" t="str">
+        <f>C70</f>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="2" t="str">
+        <f t="shared" ref="C72:C84" si="5">C71</f>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <f t="shared" si="4"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <f t="shared" si="4"/>
+        <v>74</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="7">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="7">
+        <f t="shared" si="4"/>
+        <v>79</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
+        <f t="shared" si="4"/>
+        <v>82</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
+        <f t="shared" si="4"/>
+        <v>83</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Conjunto Residencial Pq da Figureira</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+      <c r="B85" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="C85" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
+      <c r="B86" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B86" s="3" t="str">
-        <f>B85</f>
+      <c r="C86" s="2" t="str">
+        <f>C85</f>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="B87" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B87" s="3" t="str">
-        <f t="shared" ref="B87:B91" si="4">B86</f>
+      <c r="C87" s="2" t="str">
+        <f t="shared" ref="C87:C91" si="6">C86</f>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
+        <f t="shared" si="4"/>
+        <v>87</v>
+      </c>
+      <c r="B88" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B92" s="3" t="str">
-        <f>B91</f>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B93" s="3" t="str">
-        <f t="shared" ref="B93:B103" si="5">B92</f>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B95" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B97" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B98" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B99" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B100" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B101" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B102" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B103" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B104" s="3" t="str">
-        <f>B103</f>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B105" s="3" t="str">
-        <f t="shared" ref="B105:B121" si="6">B104</f>
-        <v>Encosta do Morro</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B106" s="3" t="str">
+      <c r="C88" s="2" t="str">
         <f t="shared" si="6"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B107" s="3" t="str">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
+        <f t="shared" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="2" t="str">
         <f t="shared" si="6"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B108" s="3" t="str">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
+        <f t="shared" si="4"/>
+        <v>89</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="2" t="str">
         <f t="shared" si="6"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B109" s="3" t="str">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C91" s="2" t="str">
         <f t="shared" si="6"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="2" t="str">
+        <f>C91</f>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
+        <f t="shared" si="4"/>
+        <v>92</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="2" t="str">
+        <f t="shared" ref="C93:C103" si="7">C92</f>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="B94" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <f t="shared" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="B98" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <f t="shared" si="4"/>
+        <v>101</v>
+      </c>
+      <c r="B102" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="7">
+        <f t="shared" si="4"/>
+        <v>102</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
+        <f t="shared" si="4"/>
+        <v>103</v>
+      </c>
+      <c r="B104" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B110" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C104" s="2" t="str">
+        <f>C103</f>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="7">
+        <f t="shared" si="4"/>
+        <v>104</v>
+      </c>
+      <c r="B105" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B111" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C105" s="2" t="str">
+        <f t="shared" ref="C105:C121" si="8">C104</f>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="7">
+        <f t="shared" si="4"/>
+        <v>105</v>
+      </c>
+      <c r="B106" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B112" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C106" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="7">
+        <f t="shared" si="4"/>
+        <v>106</v>
+      </c>
+      <c r="B107" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B113" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C107" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="7">
+        <f t="shared" si="4"/>
+        <v>107</v>
+      </c>
+      <c r="B108" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B114" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C108" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="7">
+        <f t="shared" si="4"/>
+        <v>108</v>
+      </c>
+      <c r="B109" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B115" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C109" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="7">
+        <f t="shared" si="4"/>
+        <v>109</v>
+      </c>
+      <c r="B110" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B116" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C110" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="7">
+        <f t="shared" si="4"/>
+        <v>110</v>
+      </c>
+      <c r="B111" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B117" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C111" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="7">
+        <f t="shared" si="4"/>
+        <v>111</v>
+      </c>
+      <c r="B112" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B118" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C112" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="7">
+        <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
+      <c r="B113" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B119" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C113" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="7">
+        <f t="shared" si="4"/>
+        <v>113</v>
+      </c>
+      <c r="B114" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B120" s="3" t="str">
-        <f t="shared" si="6"/>
+      <c r="C114" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="7">
+        <f t="shared" si="4"/>
+        <v>114</v>
+      </c>
+      <c r="B115" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B121" s="5" t="str">
-        <f t="shared" si="6"/>
+      <c r="C115" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="7">
+        <f t="shared" si="4"/>
+        <v>115</v>
+      </c>
+      <c r="B116" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C116" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="7">
+        <f t="shared" si="4"/>
+        <v>116</v>
+      </c>
+      <c r="B117" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C117" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="7">
+        <f t="shared" si="4"/>
+        <v>117</v>
+      </c>
+      <c r="B118" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="7">
+        <f t="shared" si="4"/>
+        <v>118</v>
+      </c>
+      <c r="B119" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="7">
+        <f t="shared" si="4"/>
+        <v>119</v>
+      </c>
+      <c r="B120" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Encosta do Morro</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="9">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+      <c r="B121" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>Encosta do Morro</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E18:H18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5584,129 +6092,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11">
-        <f>COUNTIF('Dados Brutos'!A2:A41,"Nenhum Grau Completo")</f>
+      <c r="B2" s="8">
+        <f>COUNTIF('Dados Brutos'!B2:B41,"Nenhum Grau Completo")</f>
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="11">
-        <f>COUNTIF('Dados Brutos'!A2:A41,"Primeiro Grau Completo")</f>
+      <c r="B3" s="8">
+        <f>COUNTIF('Dados Brutos'!B2:B41,"Primeiro Grau Completo")</f>
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11">
-        <f>COUNTIF('Dados Brutos'!A2:A41,"Segundo Grau Completo")</f>
+      <c r="B4" s="8">
+        <f>COUNTIF('Dados Brutos'!B2:B41,"Segundo Grau Completo")</f>
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="10">
         <f>SUM(B2:B4)</f>
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="32"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="11">
-        <f>COUNTIF('Dados Brutos'!A42:A84,"Nenhum Grau Completo")</f>
+      <c r="B17" s="8">
+        <f>COUNTIF('Dados Brutos'!B42:B84,"Nenhum Grau Completo")</f>
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="11">
-        <f>COUNTIF('Dados Brutos'!A42:A84,"Primeiro Grau Completo")</f>
+      <c r="B18" s="8">
+        <f>COUNTIF('Dados Brutos'!B42:B84,"Primeiro Grau Completo")</f>
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="11">
-        <f>COUNTIF('Dados Brutos'!A42:A84,"Segundo Grau Completo")</f>
+      <c r="B19" s="8">
+        <f>COUNTIF('Dados Brutos'!B42:B84,"Segundo Grau Completo")</f>
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="10">
         <f>SUM(B17:B19)</f>
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="32"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="11">
-        <f>COUNTIF('Dados Brutos'!A85:A121,"Nenhum Grau Completo")</f>
+      <c r="B29" s="8">
+        <f>COUNTIF('Dados Brutos'!B85:B121,"Nenhum Grau Completo")</f>
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="11">
-        <f>COUNTIF('Dados Brutos'!A85:A121,"Primeiro Grau Completo")</f>
+      <c r="B30" s="8">
+        <f>COUNTIF('Dados Brutos'!B85:B121,"Primeiro Grau Completo")</f>
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="11">
-        <f>COUNTIF('Dados Brutos'!A84:A121,"Segundo Grau Completo")</f>
+      <c r="B31" s="8">
+        <f>COUNTIF('Dados Brutos'!B84:B121,"Segundo Grau Completo")</f>
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="10">
         <f>SUM(B29:B31)</f>
         <v>37</v>
       </c>

</xml_diff>